<commit_message>
Fix vaccine for scale. Add some notes about scaling.
</commit_message>
<xml_diff>
--- a/Vic TB Elim Economic Models/VIC JAN/Output/R calculate test 1/working.xlsx
+++ b/Vic TB Elim Economic Models/VIC JAN/Output/R calculate test 1/working.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Repos\COVIDModel_PI\Vic TB Elim Economic Models\VIC JAN\Output\R calculate test 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC686EAF-0CE4-4AED-A091-0CDAD059314B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1B7F93-745D-4DCB-9479-4EABD67976FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29835" yWindow="1980" windowWidth="22935" windowHeight="14310" xr2:uid="{BF9210A4-B3A3-478D-9A7A-EA7E7879A04A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BF9210A4-B3A3-478D-9A7A-EA7E7879A04A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,32 +33,8 @@
     <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$T$9:$T$108</definedName>
     <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$U$8</definedName>
     <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$U$9:$U$108</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$J$8</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$J$9:$J$108</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$K$8</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$K$9:$K$108</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$L$8</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$L$9:$L$108</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$K$9:$K$108</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$M$8</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$M$9:$M$108</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$N$8</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$N$9:$N$108</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$O$8</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$O$9:$O$108</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$P$8</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$P$9:$P$108</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Sheet1!$Q$8</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Sheet1!$Q$9:$Q$108</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$L$8</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Sheet1!$R$8</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Sheet1!$R$9:$R$108</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Sheet1!$S$8</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Sheet1!$S$9:$S$108</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Sheet1!$T$8</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Sheet1!$T$9:$T$108</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">Sheet1!$U$8</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">Sheet1!$U$9:$U$108</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$L$9:$L$108</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$M$8</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$M$9:$M$108</definedName>
@@ -84,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>average_R</t>
   </si>
@@ -150,6 +126,15 @@
   </si>
   <si>
     <t>R Increase</t>
+  </si>
+  <si>
+    <t>Desired R</t>
+  </si>
+  <si>
+    <t>global_trans</t>
+  </si>
+  <si>
+    <t>Mean across runs</t>
   </si>
 </sst>
 </file>
@@ -1378,10 +1363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B9BEE34-2485-4778-83FD-7E708070F85D}">
-  <dimension ref="B1:U1201"/>
+  <dimension ref="B1:Y1201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,9 +1377,10 @@
     <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="10" max="21" width="9.85546875" customWidth="1"/>
+    <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1408,7 +1394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>2.065217391</v>
       </c>
@@ -1461,7 +1447,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1.9541284400000001</v>
       </c>
@@ -1513,8 +1499,11 @@
       <c r="U3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="W3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2.3047619049999999</v>
       </c>
@@ -1566,8 +1555,17 @@
       <c r="U4">
         <v>0.375</v>
       </c>
-    </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="W4">
+        <v>0.24</v>
+      </c>
+      <c r="X4">
+        <v>0.3</v>
+      </c>
+      <c r="Y4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1.591836735</v>
       </c>
@@ -1584,55 +1582,67 @@
         <v>18</v>
       </c>
       <c r="J5">
-        <f>AVERAGE(J9:J108)</f>
+        <f t="shared" ref="J5:U5" si="0">AVERAGE(J9:J108)</f>
         <v>2.0404152331700005</v>
       </c>
       <c r="K5">
-        <f>AVERAGE(K9:K108)</f>
+        <f t="shared" si="0"/>
         <v>2.4091424012299996</v>
       </c>
       <c r="L5">
-        <f>AVERAGE(L9:L108)</f>
+        <f t="shared" si="0"/>
         <v>2.9453157718699998</v>
       </c>
       <c r="M5">
-        <f>AVERAGE(M9:M108)</f>
+        <f t="shared" si="0"/>
         <v>2.0405434339499999</v>
       </c>
       <c r="N5">
-        <f>AVERAGE(N9:N108)</f>
+        <f t="shared" si="0"/>
         <v>2.4359834521599995</v>
       </c>
       <c r="O5">
-        <f>AVERAGE(O9:O108)</f>
+        <f t="shared" si="0"/>
         <v>2.9644673616900001</v>
       </c>
       <c r="P5">
-        <f>AVERAGE(P9:P108)</f>
+        <f t="shared" si="0"/>
         <v>2.0285022022300012</v>
       </c>
       <c r="Q5">
-        <f>AVERAGE(Q9:Q108)</f>
+        <f t="shared" si="0"/>
         <v>2.3925735504399994</v>
       </c>
       <c r="R5">
-        <f>AVERAGE(R9:R108)</f>
+        <f t="shared" si="0"/>
         <v>2.9708488840300005</v>
       </c>
       <c r="S5">
-        <f>AVERAGE(S9:S108)</f>
+        <f t="shared" si="0"/>
         <v>2.0276716682099991</v>
       </c>
       <c r="T5">
-        <f>AVERAGE(T9:T108)</f>
+        <f t="shared" si="0"/>
         <v>2.4105415122800009</v>
       </c>
       <c r="U5">
-        <f>AVERAGE(U9:U108)</f>
+        <f t="shared" si="0"/>
         <v>2.9951150709799998</v>
       </c>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="W5">
+        <f>AVERAGE(J5,M5,P5,S5)</f>
+        <v>2.0342831343900003</v>
+      </c>
+      <c r="X5">
+        <f>AVERAGE(K5,N5,Q5,T5)</f>
+        <v>2.4120602290274995</v>
+      </c>
+      <c r="Y5">
+        <f>AVERAGE(L5,O5,R5,U5)</f>
+        <v>2.9689367721424995</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1.9126213590000001</v>
       </c>
@@ -1649,55 +1659,55 @@
         <v>19</v>
       </c>
       <c r="J6">
-        <f>_xlfn.STDEV.S(J9:J108)</f>
+        <f t="shared" ref="J6:U6" si="1">_xlfn.STDEV.S(J9:J108)</f>
         <v>0.20281614462595834</v>
       </c>
       <c r="K6">
-        <f>_xlfn.STDEV.S(K9:K108)</f>
+        <f t="shared" si="1"/>
         <v>0.24837692591364571</v>
       </c>
       <c r="L6">
-        <f>_xlfn.STDEV.S(L9:L108)</f>
+        <f t="shared" si="1"/>
         <v>0.37748827301134308</v>
       </c>
       <c r="M6">
-        <f>_xlfn.STDEV.S(M9:M108)</f>
+        <f t="shared" si="1"/>
         <v>0.22525891386236008</v>
       </c>
       <c r="N6">
-        <f>_xlfn.STDEV.S(N9:N108)</f>
+        <f t="shared" si="1"/>
         <v>0.2835183115534986</v>
       </c>
       <c r="O6">
-        <f>_xlfn.STDEV.S(O9:O108)</f>
+        <f t="shared" si="1"/>
         <v>0.41586825988913578</v>
       </c>
       <c r="P6">
-        <f>_xlfn.STDEV.S(P9:P108)</f>
+        <f t="shared" si="1"/>
         <v>0.21058513161677483</v>
       </c>
       <c r="Q6">
-        <f>_xlfn.STDEV.S(Q9:Q108)</f>
+        <f t="shared" si="1"/>
         <v>0.29059648579801861</v>
       </c>
       <c r="R6">
-        <f>_xlfn.STDEV.S(R9:R108)</f>
+        <f t="shared" si="1"/>
         <v>0.36503874210905185</v>
       </c>
       <c r="S6">
-        <f>_xlfn.STDEV.S(S9:S108)</f>
+        <f t="shared" si="1"/>
         <v>0.20251159193190715</v>
       </c>
       <c r="T6">
-        <f>_xlfn.STDEV.S(T9:T108)</f>
+        <f t="shared" si="1"/>
         <v>0.28108859429788258</v>
       </c>
       <c r="U6">
-        <f>_xlfn.STDEV.S(U9:U108)</f>
+        <f t="shared" si="1"/>
         <v>0.41338538989177681</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1.971962617</v>
       </c>
@@ -1722,31 +1732,31 @@
         <v>1.2225577742379423</v>
       </c>
       <c r="N7">
-        <f t="shared" ref="M7:U7" si="0">N5/M5</f>
+        <f t="shared" ref="N7:U7" si="2">N5/M5</f>
         <v>1.1937915222145128</v>
       </c>
       <c r="O7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.2169488914472679</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.1794779161736981</v>
       </c>
       <c r="R7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.2416959484834458</v>
       </c>
       <c r="T7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.1888224065427684</v>
       </c>
       <c r="U7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.2425071527380926</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2.2234042550000002</v>
       </c>
@@ -1798,8 +1808,14 @@
       <c r="U8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>1.835616438</v>
       </c>
@@ -1851,8 +1867,15 @@
       <c r="U9">
         <v>3.30952381</v>
       </c>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X9">
+        <v>2.5</v>
+      </c>
+      <c r="Y9">
+        <f>($Y$4-$X$4)*(X9-$X$5)/($Y$5-$X$5)+$X4</f>
+        <v>0.31184370737909767</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2.1047619050000002</v>
       </c>
@@ -1901,8 +1924,15 @@
       <c r="U10">
         <v>2.92</v>
       </c>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X10">
+        <v>3</v>
+      </c>
+      <c r="Y10">
+        <f>($Y$4-$X$4)*(X10-$X$5)/($Y$5-$X$5)+$X$4</f>
+        <v>0.37918358811861719</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2.2872340430000002</v>
       </c>
@@ -1952,7 +1982,7 @@
         <v>3.2452830189999999</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>1.9523809519999999</v>
       </c>
@@ -2002,7 +2032,7 @@
         <v>3.5272727270000002</v>
       </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>2.1271186439999998</v>
       </c>
@@ -2052,7 +2082,7 @@
         <v>2.736842105</v>
       </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2.138888889</v>
       </c>
@@ -2102,7 +2132,7 @@
         <v>3.0689655170000001</v>
       </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>1.9487179489999999</v>
       </c>
@@ -2152,7 +2182,7 @@
         <v>4.3684210529999996</v>
       </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>1.97</v>
       </c>

</xml_diff>